<commit_message>
alternative approach for db storing
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -77,18 +77,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,16 +165,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G4" headerRowCount="1">
-  <autoFilter ref="A1:G4"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Montant"/>
-    <tableColumn id="2" name="Devise"/>
-    <tableColumn id="3" name="FILIALE"/>
-    <tableColumn id="4" name="Transaction Date"/>
-    <tableColumn id="5" name="ARN"/>
-    <tableColumn id="6" name="Autorisation"/>
-    <tableColumn id="7" name="Description"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L1" headerRowCount="1">
+  <autoFilter ref="A1:L1"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="FILIALE"/>
+    <tableColumn id="2" name="Réseau"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="Devise"/>
+    <tableColumn id="6" name="Nbre Total De Transactions"/>
+    <tableColumn id="7" name="Montant Total de Transactions"/>
+    <tableColumn id="8" name="Montant de Transactions (Couverture)"/>
+    <tableColumn id="9" name="Nbre Total de Rejets"/>
+    <tableColumn id="10" name="Nbre de Transactions (Couverture)"/>
+    <tableColumn id="11" name="Rapprochement"/>
+    <tableColumn id="12" name="Montant de Rejets"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -470,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,158 +484,77 @@
   <cols>
     <col width="9" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="297" customWidth="1" min="7" max="7"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="6" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
+    <col width="31" customWidth="1" min="7" max="7"/>
+    <col width="38" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="35" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="19" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Montant</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
+          <t>FILIALE</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Réseau</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Devise</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>FILIALE</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Transaction Date</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>ARN</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Autorisation</t>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre Total De Transactions</t>
         </is>
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>84,000</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>XOF</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>SG - COTE D IVOIRE</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>72681594150101332418418</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>059369</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000118 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000118 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>25,000</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>XOF</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>SG - COTE D IVOIRE</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>72681594150101332421271</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>059347</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000124 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000124 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>435,000</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>XOF</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>SG - COTE D IVOIRE</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>72681594150101332383190</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>059403</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000258 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000258 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+          <t>Montant Total de Transactions</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Montant de Transactions (Couverture)</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre Total de Rejets</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre de Transactions (Couverture)</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Rapprochement</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>Montant de Rejets</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Transalation to french for better Ux
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -77,17 +77,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -165,21 +166,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L1" headerRowCount="1">
-  <autoFilter ref="A1:L1"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="FILIALE"/>
-    <tableColumn id="2" name="Réseau"/>
-    <tableColumn id="3" name="Type"/>
-    <tableColumn id="4" name="Date"/>
-    <tableColumn id="5" name="Devise"/>
-    <tableColumn id="6" name="Nbre Total De Transactions"/>
-    <tableColumn id="7" name="Montant Total de Transactions"/>
-    <tableColumn id="8" name="Montant de Transactions (Couverture)"/>
-    <tableColumn id="9" name="Nbre Total de Rejets"/>
-    <tableColumn id="10" name="Nbre de Transactions (Couverture)"/>
-    <tableColumn id="11" name="Rapprochement"/>
-    <tableColumn id="12" name="Montant de Rejets"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G4" headerRowCount="1">
+  <autoFilter ref="A1:G4"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Montant"/>
+    <tableColumn id="2" name="Devise"/>
+    <tableColumn id="3" name="FILIALE"/>
+    <tableColumn id="4" name="Transaction Date"/>
+    <tableColumn id="5" name="ARN"/>
+    <tableColumn id="6" name="Autorisation"/>
+    <tableColumn id="7" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -474,7 +470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,77 +480,158 @@
   <cols>
     <col width="9" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="6" customWidth="1" min="4" max="4"/>
-    <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="28" customWidth="1" min="6" max="6"/>
-    <col width="31" customWidth="1" min="7" max="7"/>
-    <col width="38" customWidth="1" min="8" max="8"/>
-    <col width="22" customWidth="1" min="9" max="9"/>
-    <col width="35" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="19" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="297" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
+          <t>Montant</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Devise</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
           <t>FILIALE</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Réseau</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Devise</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Nbre Total De Transactions</t>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Transaction Date</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>ARN</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Autorisation</t>
         </is>
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>Montant Total de Transactions</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>Montant de Transactions (Couverture)</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>Nbre Total de Rejets</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
-        <is>
-          <t>Nbre de Transactions (Couverture)</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>Rapprochement</t>
-        </is>
-      </c>
-      <c r="L1" s="3" t="inlineStr">
-        <is>
-          <t>Montant de Rejets</t>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>84,000</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>72681594150101332418418</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>059369</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000118 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000118 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>25,000</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>72681594150101332421271</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>059347</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000124 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000124 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>435,000</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>72681594150101332383190</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>059403</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000258 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000258 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
reformating of df_rejections as asked
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -82,10 +82,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -166,16 +166,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G4" headerRowCount="1">
-  <autoFilter ref="A1:G4"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Montant"/>
-    <tableColumn id="2" name="Devise"/>
-    <tableColumn id="3" name="FILIALE"/>
-    <tableColumn id="4" name="Transaction Date"/>
-    <tableColumn id="5" name="ARN"/>
-    <tableColumn id="6" name="Autorisation"/>
-    <tableColumn id="7" name="Description"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H4" headerRowCount="1">
+  <autoFilter ref="A1:H4"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="FILIALE"/>
+    <tableColumn id="2" name="RESEAU"/>
+    <tableColumn id="3" name="ARN"/>
+    <tableColumn id="4" name="Autorisation"/>
+    <tableColumn id="5" name="Date Transaction"/>
+    <tableColumn id="6" name="Montant"/>
+    <tableColumn id="7" name="Devise"/>
+    <tableColumn id="8" name="Motif"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -470,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,158 +479,179 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="297" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="26" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="297" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
+          <t>FILIALE</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>RESEAU</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>ARN</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Autorisation</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Date Transaction</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
           <t>Montant</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Devise</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>FILIALE</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Transaction Date</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>ARN</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Autorisation</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Motif</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>72681594150101332418418</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>059369</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>84,000</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>SG - COTE D IVOIRE</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>72681594150101332418418</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>059369</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000118 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000118 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>72681594150101332421271</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>059347</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>25,000</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>SG - COTE D IVOIRE</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>72681594150101332421271</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>059347</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000124 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000124 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>72681594150101332383190</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>059403</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
         <is>
           <t>435,000</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>SG - COTE D IVOIRE</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>72681594150101332383190</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>059403</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000258 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000258 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
         </is>

</xml_diff>

<commit_message>
calendar and cards changes along with some other minor changes
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,6 +35,9 @@
     <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -77,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -89,6 +92,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,17 +170,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H4" headerRowCount="1">
-  <autoFilter ref="A1:H4"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L13" headerRowCount="1">
+  <autoFilter ref="A1:L13"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="FILIALE"/>
-    <tableColumn id="2" name="RESEAU"/>
-    <tableColumn id="3" name="ARN"/>
-    <tableColumn id="4" name="Autorisation"/>
-    <tableColumn id="5" name="Date Transaction"/>
-    <tableColumn id="6" name="Montant"/>
-    <tableColumn id="7" name="Devise"/>
-    <tableColumn id="8" name="Motif"/>
+    <tableColumn id="2" name="Réseau"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="Devise"/>
+    <tableColumn id="6" name="Nbre Total De Transactions"/>
+    <tableColumn id="7" name="Montant Total de Transactions"/>
+    <tableColumn id="8" name="Montant de Rejets"/>
+    <tableColumn id="9" name="Nbre Total de Rejets"/>
+    <tableColumn id="10" name="Rapprochement"/>
+    <tableColumn id="11" name="Nbre de Transactions (Couverture)"/>
+    <tableColumn id="12" name="Montant de Transactions (Couverture)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -471,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,14 +487,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="297" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
+    <col width="31" customWidth="1" min="7" max="7"/>
+    <col width="19" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="35" customWidth="1" min="11" max="11"/>
+    <col width="38" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -497,44 +509,64 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>RESEAU</t>
+          <t>Réseau</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>ARN</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Autorisation</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Date Transaction</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Montant</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
           <t>Devise</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Motif</t>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre Total De Transactions</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Montant Total de Transactions</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Montant de Rejets</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre Total de Rejets</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Rapprochement</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre de Transactions (Couverture)</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>Montant de Transactions (Couverture)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SG - COTE D IVOIRE</t>
+          <t>SG - BENIN</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -542,41 +574,43 @@
           <t>MASTERCARD INTERNATIONAL</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>72681594150101332418418</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>059369</t>
+          <t>2024-01-17</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>84,000</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000118 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000118 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>61,760.00</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="n"/>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="inlineStr">
+        <is>
+          <t>61,760.00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SG - COTE D IVOIRE</t>
+          <t>SG - BENIN</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -586,74 +620,529 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>72681594150101332421271</t>
+          <t>ACHAT</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>059347</t>
+          <t>2024-01-17</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>25,000</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000124 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000124 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+      <c r="F3" t="n">
+        <v>52</v>
+      </c>
+      <c r="G3" s="4" t="inlineStr">
+        <is>
+          <t>2,517,189.00</t>
+        </is>
+      </c>
+      <c r="H3" s="4" t="n"/>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>52</v>
+      </c>
+      <c r="L3" s="4" t="inlineStr">
+        <is>
+          <t>2,517,189.00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>SG - BURKINA FASO</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>625,398.00</t>
+        </is>
+      </c>
+      <c r="H4" s="4" t="n"/>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>8</v>
+      </c>
+      <c r="L4" s="4" t="inlineStr">
+        <is>
+          <t>625,398.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SG - CAMEROUN</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>XAF</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>105</v>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>8,233,671.00</t>
+        </is>
+      </c>
+      <c r="H5" s="4" t="n"/>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>105</v>
+      </c>
+      <c r="L5" s="4" t="inlineStr">
+        <is>
+          <t>8,233,671.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>SG - COTE D IVOIRE</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>MASTERCARD INTERNATIONAL</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>72681594150101332383190</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>059403</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="inlineStr">
-        <is>
-          <t>435,000</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000258 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000258 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+      <c r="F6" t="n">
+        <v>324</v>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>48,010,154.00</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="n"/>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>324</v>
+      </c>
+      <c r="L6" s="4" t="inlineStr">
+        <is>
+          <t>48,010,154.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SG - GUINEE CONAKRY</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>GNF</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>23</v>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>30,950,095.00</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="n"/>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>23</v>
+      </c>
+      <c r="L7" s="4" t="inlineStr">
+        <is>
+          <t>30,950,095.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SG - GUINEE EQUATORIALE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>XAF</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>13</v>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>877,829.00</t>
+        </is>
+      </c>
+      <c r="H8" s="4" t="n"/>
+      <c r="J8" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L8" s="4" t="inlineStr">
+        <is>
+          <t>877,829.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SG - MADAGASCAR</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>36</v>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>2,238.45</t>
+        </is>
+      </c>
+      <c r="H9" s="4" t="n"/>
+      <c r="J9" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>36</v>
+      </c>
+      <c r="L9" s="4" t="inlineStr">
+        <is>
+          <t>2,238.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SG - MADAGASCAR</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MGA</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>188</v>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>70,578,636.10</t>
+        </is>
+      </c>
+      <c r="H10" s="4" t="n"/>
+      <c r="J10" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>188</v>
+      </c>
+      <c r="L10" s="4" t="inlineStr">
+        <is>
+          <t>70,578,636.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SG - MADAGASCAR</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CASH ADVANCE</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MGA</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>24,000,000.00</t>
+        </is>
+      </c>
+      <c r="H11" s="4" t="n"/>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>5</v>
+      </c>
+      <c r="L11" s="4" t="inlineStr">
+        <is>
+          <t>24,000,000.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SG - SENEGAL</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>254</v>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>36,602,175.00</t>
+        </is>
+      </c>
+      <c r="H12" s="4" t="n"/>
+      <c r="J12" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>254</v>
+      </c>
+      <c r="L12" s="4" t="inlineStr">
+        <is>
+          <t>36,602,175.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SG - TCHAD</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2024-01-17</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>XAF</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>597,000.00</t>
+        </is>
+      </c>
+      <c r="H13" s="4" t="n"/>
+      <c r="J13" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>4</v>
+      </c>
+      <c r="L13" s="4" t="inlineStr">
+        <is>
+          <t>597,000.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding transactionrecyclees to the pie chart
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -557,10 +557,8 @@
           <t>2024-05-28</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>84,000</t>
-        </is>
+      <c r="F2" s="4" t="n">
+        <v>84000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -599,10 +597,8 @@
           <t>2024-05-28</t>
         </is>
       </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>25,000</t>
-        </is>
+      <c r="F3" s="4" t="n">
+        <v>25000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -641,10 +637,8 @@
           <t>2024-05-28</t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
-        <is>
-          <t>435,000</t>
-        </is>
+      <c r="F4" s="4" t="n">
+        <v>435000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fix of bug that merges twice the recyled dataframe
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,6 +35,9 @@
     <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -77,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -89,6 +92,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,17 +170,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H4" headerRowCount="1">
-  <autoFilter ref="A1:H4"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L13" headerRowCount="1">
+  <autoFilter ref="A1:L13"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="FILIALE"/>
-    <tableColumn id="2" name="RESEAU"/>
-    <tableColumn id="3" name="ARN"/>
-    <tableColumn id="4" name="Autorisation"/>
-    <tableColumn id="5" name="Date Transaction"/>
-    <tableColumn id="6" name="Montant"/>
-    <tableColumn id="7" name="Devise"/>
-    <tableColumn id="8" name="Motif"/>
+    <tableColumn id="2" name="Réseau"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="Devise"/>
+    <tableColumn id="6" name="Nbre Total De Transactions"/>
+    <tableColumn id="7" name="Montant Total de Transactions"/>
+    <tableColumn id="8" name="Montant de Transactions (Couverture)"/>
+    <tableColumn id="9" name="Rapprochement"/>
+    <tableColumn id="10" name="Montant de Rejets"/>
+    <tableColumn id="11" name="Nbre Total de Rejets"/>
+    <tableColumn id="12" name="Nbre de Transactions (Couverture)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -471,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,14 +487,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="297" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
+    <col width="31" customWidth="1" min="7" max="7"/>
+    <col width="38" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="19" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="35" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -497,44 +509,64 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>RESEAU</t>
+          <t>Réseau</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>ARN</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Autorisation</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Date Transaction</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Montant</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
           <t>Devise</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Motif</t>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre Total De Transactions</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Montant Total de Transactions</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Montant de Transactions (Couverture)</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Rapprochement</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>Montant de Rejets</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre Total de Rejets</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Nbre de Transactions (Couverture)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SG - COTE D IVOIRE</t>
+          <t>SG - BENIN</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -544,37 +576,46 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>72681594150101332418418</t>
+          <t>ACHAT</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>059369</t>
+          <t>2024-07-01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>84000</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000118 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000118 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
-        </is>
+      <c r="F2" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>2,388,416.00</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="inlineStr">
+        <is>
+          <t>2,388,416.00</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J2" s="4" t="n"/>
+      <c r="L2" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SG - COTE D IVOIRE</t>
+          <t>SG - BURKINA FASO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -584,71 +625,525 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>72681594150101332421271</t>
+          <t>ACHAT</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>059347</t>
+          <t>2024-07-01</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>25000</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000124 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000124 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
-        </is>
+      <c r="F3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4" t="inlineStr">
+        <is>
+          <t>1,285,794.00</t>
+        </is>
+      </c>
+      <c r="H3" s="4" t="inlineStr">
+        <is>
+          <t>1,285,794.00</t>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J3" s="4" t="n"/>
+      <c r="L3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>SG - CAMEROUN</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>XAF</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>137</v>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>12,286,047.00</t>
+        </is>
+      </c>
+      <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>12,286,047.00</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J4" s="4" t="n"/>
+      <c r="L4" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>SG - COTE D IVOIRE</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>MASTERCARD INTERNATIONAL</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>72681594150101332383190</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>059403</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>435000</v>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000258 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000258 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
-        </is>
+      <c r="F5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>206,399.00</t>
+        </is>
+      </c>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>206,399.00</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J5" s="4" t="n"/>
+      <c r="L5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>250</v>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>60,883,146.00</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>60,883,146.00</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J6" s="4" t="n"/>
+      <c r="L6" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SG - GUINEE CONAKRY</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>GNF</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>54</v>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>104,391,018.00</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="inlineStr">
+        <is>
+          <t>104,391,018.00</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J7" s="4" t="n"/>
+      <c r="L7" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SG - GUINEE EQUATORIALE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>XAF</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>395,955.00</t>
+        </is>
+      </c>
+      <c r="H8" s="4" t="inlineStr">
+        <is>
+          <t>395,955.00</t>
+        </is>
+      </c>
+      <c r="I8" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J8" s="4" t="n"/>
+      <c r="L8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SG - MADAGASCAR</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>27</v>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>3,074.18</t>
+        </is>
+      </c>
+      <c r="H9" s="4" t="inlineStr">
+        <is>
+          <t>3,074.18</t>
+        </is>
+      </c>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J9" s="4" t="n"/>
+      <c r="L9" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SG - MADAGASCAR</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MGA</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>231</v>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>81,773,559.00</t>
+        </is>
+      </c>
+      <c r="H10" s="4" t="inlineStr">
+        <is>
+          <t>81,773,559.00</t>
+        </is>
+      </c>
+      <c r="I10" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J10" s="4" t="n"/>
+      <c r="L10" t="n">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SG - MADAGASCAR</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CASH ADVANCE</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MGA</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>20,900,000.00</t>
+        </is>
+      </c>
+      <c r="H11" s="4" t="inlineStr">
+        <is>
+          <t>20,900,000.00</t>
+        </is>
+      </c>
+      <c r="I11" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J11" s="4" t="n"/>
+      <c r="L11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SG - SENEGAL</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>164</v>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>20,199,614.00</t>
+        </is>
+      </c>
+      <c r="H12" s="4" t="inlineStr">
+        <is>
+          <t>20,199,614.00</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J12" s="4" t="n"/>
+      <c r="L12" t="n">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SG - TCHAD</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>XAF</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>9</v>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>437,050.00</t>
+        </is>
+      </c>
+      <c r="H13" s="4" t="inlineStr">
+        <is>
+          <t>437,050.00</t>
+        </is>
+      </c>
+      <c r="I13" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="J13" s="4" t="n"/>
+      <c r="L13" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>